<commit_message>
heb weernieuwpcastatic.py een goede standaardizatie
</commit_message>
<xml_diff>
--- a/PCAstatic/PCAstatic_predicted_factors_matrix_10.xlsx
+++ b/PCAstatic/PCAstatic_predicted_factors_matrix_10.xlsx
@@ -443,82 +443,82 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-5.546004450979949</v>
+        <v>-1.484439164362272</v>
       </c>
       <c r="B2" t="n">
-        <v>-5.34045850919005</v>
+        <v>-1.27922042006967</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-1.149301176356966</v>
+        <v>-0.4646261626649179</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.131202972523497</v>
+        <v>-0.5894678462724917</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.3394332167418996</v>
+        <v>-1.002315334143556</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.1981644286802984</v>
+        <v>-0.8420532791301936</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-1.178004393929078</v>
+        <v>-0.725020227433065</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.7595660621586662</v>
+        <v>-0.6808037628073165</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.1314775148644428</v>
+        <v>0.8211783586799222</v>
       </c>
       <c r="B6" t="n">
-        <v>0.07734033066112114</v>
+        <v>0.6820964583389857</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1983727107882802</v>
+        <v>-0.09213892798072537</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1439439259330764</v>
+        <v>0.005658836007705776</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.3506641371955279</v>
+        <v>0.7902620007208699</v>
       </c>
       <c r="B8" t="n">
-        <v>0.2380344147737066</v>
+        <v>0.6113274057277852</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.09753381730995681</v>
+        <v>0.3284874063919779</v>
       </c>
       <c r="B9" t="n">
-        <v>0.03166756318959256</v>
+        <v>0.3285947465387778</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.04731397797236764</v>
+        <v>-0.1876080986239586</v>
       </c>
       <c r="B10" t="n">
-        <v>0.03053534835443629</v>
+        <v>-0.04585113813152625</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.009430013393246088</v>
+        <v>-0.2903066199609222</v>
       </c>
       <c r="B11" t="n">
-        <v>0.003002641750018904</v>
+        <v>-0.1285775647085816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
standaardizeer nu de rijen ipv kolommen, en gebruik de mean en sd van Y_train om Y_validate mee te standaardizeren Factoren divergeren nu enorm, gaat nor ergens fout!
</commit_message>
<xml_diff>
--- a/PCAstatic/PCAstatic_predicted_factors_matrix_10.xlsx
+++ b/PCAstatic/PCAstatic_predicted_factors_matrix_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,13 +440,115 @@
       <c r="B1" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>-1.484439164362272</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.27922042006967</v>
+        <v>-123.9550296711438</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3380.890217572635</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-968611.9862105123</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-328301487.2324842</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-92848107320.68393</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-27841850607351.39</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-8274136495356425</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-2.418411949167883e+18</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-6.839402871410957e+20</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-1.85923150426396e+23</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-4.888926956790534e+25</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-1.254396324365021e+28</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-3.170602458665152e+30</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-7.923746820402575e+32</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-1.960530415155599e+35</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-4.817802141023544e+37</v>
+      </c>
+      <c r="R2" t="n">
+        <v>-1.180438569912226e+40</v>
+      </c>
+      <c r="S2" t="n">
+        <v>-2.891479340731916e+42</v>
       </c>
     </row>
     <row r="3">
@@ -454,7 +556,58 @@
         <v>-0.4646261626649179</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.5894678462724917</v>
+        <v>-86.50748073891744</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-21199.62476671857</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-3804048.817149667</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-727886835.3080769</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-146240537256.1685</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-29921187127535.09</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-5871319052448512</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.138773065010225e+18</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.176600620732487e+20</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4.063778692347121e+22</v>
+      </c>
+      <c r="L3" t="n">
+        <v>7.294871106833389e+24</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1.227799467987582e+27</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1.860413033280916e+29</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2.370111096315683e+31</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2.196445611748111e+33</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>7.912019788770446e+34</v>
+      </c>
+      <c r="R3" t="n">
+        <v>-1.515331604447711e+37</v>
+      </c>
+      <c r="S3" t="n">
+        <v>-3.604019181248221e+39</v>
       </c>
     </row>
     <row r="4">
@@ -462,7 +615,58 @@
         <v>-1.002315334143556</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.8420532791301936</v>
+        <v>-23.7945229249472</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-1133.715004365023</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-109012.3201676904</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-14786012.21501993</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-5010064455.69026</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-1809102744010.896</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-305282315639221.1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-5.197771661588534e+16</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-7.522129434636428e+18</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-6.69257228155166e+20</v>
+      </c>
+      <c r="L4" t="n">
+        <v>4.297277380893128e+22</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3.353546725951444e+25</v>
+      </c>
+      <c r="N4" t="n">
+        <v>7.611986338547318e+27</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1.054433485119988e+30</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1.504764434057607e+32</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2.450196958327342e+34</v>
+      </c>
+      <c r="R4" t="n">
+        <v>4.382243552268439e+36</v>
+      </c>
+      <c r="S4" t="n">
+        <v>8.563176197449328e+38</v>
       </c>
     </row>
     <row r="5">
@@ -470,7 +674,58 @@
         <v>-0.725020227433065</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.6808037628073165</v>
+        <v>74.53779669725925</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8980.685850769785</v>
+      </c>
+      <c r="D5" t="n">
+        <v>979199.2894152522</v>
+      </c>
+      <c r="E5" t="n">
+        <v>197623448.2133969</v>
+      </c>
+      <c r="F5" t="n">
+        <v>41025934896.37175</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8261323074037.866</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1531059161783212</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2.684637731625159e+17</v>
+      </c>
+      <c r="J5" t="n">
+        <v>4.282650695763159e+19</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-5.895551896920629e+21</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-6.522156903385652e+23</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-5.636975371537483e+25</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-5.835180986280031e+27</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-9.607670181694175e+29</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-1.564805350594818e+32</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-2.611876807852465e+34</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-4.606749158009495e+36</v>
+      </c>
+      <c r="S5" t="n">
+        <v>-8.482669007799447e+38</v>
       </c>
     </row>
     <row r="6">
@@ -478,7 +733,58 @@
         <v>0.8211783586799222</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6820964583389857</v>
+        <v>-12.09992167288656</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-3138.002594108159</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-1070453.472147528</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-147145902.7146581</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-18523181743.97122</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-1995795015540.625</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-129432522946171.3</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1052558664115006</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.396742157383479e+18</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1.97419477727929e+20</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2.612788687519724e+22</v>
+      </c>
+      <c r="M6" t="n">
+        <v>3.305990545317029e+24</v>
+      </c>
+      <c r="N6" t="n">
+        <v>4.222877141331624e+26</v>
+      </c>
+      <c r="O6" t="n">
+        <v>5.134099512207023e+28</v>
+      </c>
+      <c r="P6" t="n">
+        <v>5.613397177681693e+30</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>5.936799064206004e+32</v>
+      </c>
+      <c r="R6" t="n">
+        <v>7.388462032870837e+34</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1.17815123624061e+37</v>
       </c>
     </row>
     <row r="7">
@@ -486,7 +792,58 @@
         <v>-0.09213892798072537</v>
       </c>
       <c r="B7" t="n">
-        <v>0.005658836007705776</v>
+        <v>-0.5780088460346426</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3246.844812184865</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-703584.2465934869</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-117855349.9274273</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-18151156532.72955</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-2521533639397.003</v>
+      </c>
+      <c r="H7" t="n">
+        <v>269724407287015.3</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.550275162196206e+16</v>
+      </c>
+      <c r="J7" t="n">
+        <v>3.686577775503455e+17</v>
+      </c>
+      <c r="K7" t="n">
+        <v>3.291634512405745e+19</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.846332648638027e+21</v>
+      </c>
+      <c r="M7" t="n">
+        <v>6.217029979843464e+22</v>
+      </c>
+      <c r="N7" t="n">
+        <v>4.517927202320752e+25</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1.998924911244e+28</v>
+      </c>
+      <c r="P7" t="n">
+        <v>5.247490783514707e+30</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>1.089123249415757e+33</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1.944616400972955e+35</v>
+      </c>
+      <c r="S7" t="n">
+        <v>3.199637527639266e+37</v>
       </c>
     </row>
     <row r="8">
@@ -494,7 +851,58 @@
         <v>0.7902620007208699</v>
       </c>
       <c r="B8" t="n">
-        <v>0.6113274057277852</v>
+        <v>55.13059294885095</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5569.808360804794</v>
+      </c>
+      <c r="D8" t="n">
+        <v>614515.2166537135</v>
+      </c>
+      <c r="E8" t="n">
+        <v>97794724.43318053</v>
+      </c>
+      <c r="F8" t="n">
+        <v>14392652762.03738</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1690019364860.593</v>
+      </c>
+      <c r="H8" t="n">
+        <v>117256402342478.9</v>
+      </c>
+      <c r="I8" t="n">
+        <v>5339347734263029</v>
+      </c>
+      <c r="J8" t="n">
+        <v>7.288863790067747e+17</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1.040662000720591e+20</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1.454625526021431e+22</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.99452226127091e+24</v>
+      </c>
+      <c r="N8" t="n">
+        <v>2.676269763067067e+26</v>
+      </c>
+      <c r="O8" t="n">
+        <v>3.403802750445157e+28</v>
+      </c>
+      <c r="P8" t="n">
+        <v>4.156179148466393e+30</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>5.211180891825364e+32</v>
+      </c>
+      <c r="R8" t="n">
+        <v>7.309991732756115e+34</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1.143702440222433e+37</v>
       </c>
     </row>
     <row r="9">
@@ -502,7 +910,58 @@
         <v>0.3284874063919779</v>
       </c>
       <c r="B9" t="n">
-        <v>0.3285947465387778</v>
+        <v>-13.98504248671313</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3101.812342922862</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-472858.1050346395</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-52985649.50732504</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-1025142149.860469</v>
+      </c>
+      <c r="G9" t="n">
+        <v>31240597246.33014</v>
+      </c>
+      <c r="H9" t="n">
+        <v>8251754174444.872</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1239605339514720</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2.066151898169684e+17</v>
+      </c>
+      <c r="K9" t="n">
+        <v>3.060300344185169e+19</v>
+      </c>
+      <c r="L9" t="n">
+        <v>4.295117652826592e+21</v>
+      </c>
+      <c r="M9" t="n">
+        <v>5.684358737303008e+23</v>
+      </c>
+      <c r="N9" t="n">
+        <v>7.102216109934127e+25</v>
+      </c>
+      <c r="O9" t="n">
+        <v>8.507686123264285e+27</v>
+      </c>
+      <c r="P9" t="n">
+        <v>9.870293742783467e+29</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1.172100902963032e+32</v>
+      </c>
+      <c r="R9" t="n">
+        <v>1.523766484778648e+34</v>
+      </c>
+      <c r="S9" t="n">
+        <v>2.145383427017391e+36</v>
       </c>
     </row>
     <row r="10">
@@ -510,7 +969,58 @@
         <v>-0.1876080986239586</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.04585113813152625</v>
+        <v>11.71931852019795</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1500.144081287526</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-196597.1491945873</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-13233119.04195265</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-5194960458.350213</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-226655556976.6904</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-21426587610719.19</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-1499854235493524</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-9.851555236647238e+16</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-4.311300380867872e+18</v>
+      </c>
+      <c r="L10" t="n">
+        <v>6.345612406388349e+20</v>
+      </c>
+      <c r="M10" t="n">
+        <v>2.11940258401018e+23</v>
+      </c>
+      <c r="N10" t="n">
+        <v>3.764795300621928e+25</v>
+      </c>
+      <c r="O10" t="n">
+        <v>5.785386092053609e+27</v>
+      </c>
+      <c r="P10" t="n">
+        <v>8.577352875465698e+29</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>1.216809867782951e+32</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1.657663435641553e+34</v>
+      </c>
+      <c r="S10" t="n">
+        <v>2.203798982801403e+36</v>
       </c>
     </row>
     <row r="11">
@@ -518,7 +1028,58 @@
         <v>-0.2903066199609222</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.1285775647085816</v>
+        <v>-7.725247398441531</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-890.9956824164003</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-228324.4615363584</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-25731770.35797049</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-786658295.1196961</v>
+      </c>
+      <c r="G11" t="n">
+        <v>21283162417.17806</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-2924917975904.215</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-392717418081735.9</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-4.784775862809235e+16</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-5.185000143901593e+18</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-5.346423522322249e+20</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-5.32849343311675e+22</v>
+      </c>
+      <c r="N11" t="n">
+        <v>-5.393668334119915e+24</v>
+      </c>
+      <c r="O11" t="n">
+        <v>-5.725027233010528e+26</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-6.050810105784307e+28</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-6.507729295805268e+30</v>
+      </c>
+      <c r="R11" t="n">
+        <v>-7.289958299875775e+32</v>
+      </c>
+      <c r="S11" t="n">
+        <v>-8.389981121472554e+34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>